<commit_message>
update DA plan with asset smoothing
</commit_message>
<xml_diff>
--- a/Analysis/figTbl_guidebook/tbl_ERCvol.xlsx
+++ b/Analysis/figTbl_guidebook/tbl_ERCvol.xlsx
@@ -218,7 +218,7 @@
         <v>16.326620340173903</v>
       </c>
       <c r="L2" t="n">
-        <v>15.179626230283374</v>
+        <v>10.590381513073359</v>
       </c>
     </row>
     <row r="3">
@@ -256,7 +256,7 @@
         <v>13.565433698725837</v>
       </c>
       <c r="L3" t="n">
-        <v>12.896615720994511</v>
+        <v>7.436588870821143</v>
       </c>
     </row>
     <row r="4">
@@ -294,7 +294,7 @@
         <v>11.60033374861998</v>
       </c>
       <c r="L4" t="n">
-        <v>11.060873961629088</v>
+        <v>4.574353369295283</v>
       </c>
     </row>
     <row r="5">
@@ -332,7 +332,7 @@
         <v>7.690482783508735</v>
       </c>
       <c r="L5" t="n">
-        <v>8.407862702842912</v>
+        <v>2.139369966088215</v>
       </c>
     </row>
     <row r="6">
@@ -370,7 +370,7 @@
         <v>0.5549766187341015</v>
       </c>
       <c r="L6" t="n">
-        <v>4.359821513678734</v>
+        <v>-0.013259625588434715</v>
       </c>
     </row>
   </sheetData>
@@ -457,7 +457,7 @@
         <v>21.011485400072488</v>
       </c>
       <c r="L2" t="n">
-        <v>19.489253676388024</v>
+        <v>12.403076186331873</v>
       </c>
     </row>
     <row r="3">
@@ -495,7 +495,7 @@
         <v>17.451643563427186</v>
       </c>
       <c r="L3" t="n">
-        <v>18.262281075452684</v>
+        <v>12.604600069572124</v>
       </c>
     </row>
     <row r="4">
@@ -533,7 +533,7 @@
         <v>13.72991812162649</v>
       </c>
       <c r="L4" t="n">
-        <v>17.894739638418358</v>
+        <v>12.247200154346169</v>
       </c>
     </row>
     <row r="5">
@@ -571,7 +571,7 @@
         <v>10.012326657562749</v>
       </c>
       <c r="L5" t="n">
-        <v>14.23605324036133</v>
+        <v>8.095968115458708</v>
       </c>
     </row>
     <row r="6">
@@ -609,7 +609,7 @@
         <v>5.658507367699614</v>
       </c>
       <c r="L6" t="n">
-        <v>8.863920051953212</v>
+        <v>2.1579746505972777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update results for DA with asset smoothing
</commit_message>
<xml_diff>
--- a/Analysis/figTbl_guidebook/tbl_ERCvol.xlsx
+++ b/Analysis/figTbl_guidebook/tbl_ERCvol.xlsx
@@ -141,7 +141,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -218,7 +218,7 @@
         <v>16.326620340173903</v>
       </c>
       <c r="L2" t="n">
-        <v>10.590381513073359</v>
+        <v>9.68125932284621</v>
       </c>
     </row>
     <row r="3">
@@ -256,7 +256,7 @@
         <v>13.565433698725837</v>
       </c>
       <c r="L3" t="n">
-        <v>7.436588870821143</v>
+        <v>6.830689243486568</v>
       </c>
     </row>
     <row r="4">
@@ -294,7 +294,7 @@
         <v>11.60033374861998</v>
       </c>
       <c r="L4" t="n">
-        <v>4.574353369295283</v>
+        <v>4.678333523980239</v>
       </c>
     </row>
     <row r="5">
@@ -332,7 +332,7 @@
         <v>7.690482783508735</v>
       </c>
       <c r="L5" t="n">
-        <v>2.139369966088215</v>
+        <v>1.6009054314387683</v>
       </c>
     </row>
     <row r="6">
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -457,7 +457,7 @@
         <v>21.011485400072488</v>
       </c>
       <c r="L2" t="n">
-        <v>12.403076186331873</v>
+        <v>13.107931845338065</v>
       </c>
     </row>
     <row r="3">
@@ -495,7 +495,7 @@
         <v>17.451643563427186</v>
       </c>
       <c r="L3" t="n">
-        <v>12.604600069572124</v>
+        <v>12.583896662614858</v>
       </c>
     </row>
     <row r="4">
@@ -533,7 +533,7 @@
         <v>13.72991812162649</v>
       </c>
       <c r="L4" t="n">
-        <v>12.247200154346169</v>
+        <v>10.712680603328597</v>
       </c>
     </row>
     <row r="5">
@@ -571,7 +571,7 @@
         <v>10.012326657562749</v>
       </c>
       <c r="L5" t="n">
-        <v>8.095968115458708</v>
+        <v>7.7846627391028616</v>
       </c>
     </row>
     <row r="6">
@@ -609,7 +609,7 @@
         <v>5.658507367699614</v>
       </c>
       <c r="L6" t="n">
-        <v>2.1579746505972777</v>
+        <v>1.783263634148224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>